<commit_message>
Week 3 Time Management log
The following update is my timelog that is missing from my week 3 update
</commit_message>
<xml_diff>
--- a/Logs/GriffinLarry_1601_TimeManagement.xlsx
+++ b/Logs/GriffinLarry_1601_TimeManagement.xlsx
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="238" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" zoomScale="238" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -805,8 +805,12 @@
       <c r="A24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="7">
+        <v>10</v>
+      </c>
+      <c r="C24" s="7">
+        <v>10</v>
+      </c>
       <c r="D24" s="7">
         <f>B24-C24</f>
         <v>0</v>
@@ -816,33 +820,45 @@
       <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="7">
+        <v>20</v>
+      </c>
+      <c r="C25" s="7">
+        <v>15</v>
+      </c>
       <c r="D25" s="7">
         <f t="shared" ref="D25:D27" si="3">B25-C25</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="7">
+        <v>120</v>
+      </c>
+      <c r="C26" s="7">
+        <v>50</v>
+      </c>
       <c r="D26" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="7">
+        <v>20</v>
+      </c>
+      <c r="C27" s="7">
+        <v>10</v>
+      </c>
       <c r="D27" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -851,15 +867,15 @@
       </c>
       <c r="B28">
         <f>SUM(B24:B27)</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="C28">
         <f t="shared" ref="C28:D28" si="4">SUM(C24:C27)</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="D28">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>